<commit_message>
Installed pandas module and import it on the program file
</commit_message>
<xml_diff>
--- a/#2 Highest GWA Finder/students_gwa.xlsx
+++ b/#2 Highest GWA Finder/students_gwa.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flore\Desktop\BSCpE 1-2 - Second Sem\[01] CMPE 103 - Object Oriented Programming\[0000] Activities\[04] Program 4\file_handling-exercises\#2 Highest GWA Finder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
-    <sheet name="Class of 2024" sheetId="1" r:id="rId1"/>
+    <sheet name="Class of 2024" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>GWA</t>
   </si>
   <si>
@@ -90,13 +87,16 @@
   </si>
   <si>
     <t>Jessica Ho</t>
+  </si>
+  <si>
+    <t>NAME</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +110,35 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -127,64 +146,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -195,17 +200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0">
-  <autoFilter ref="A1:B21"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="GWA" dataDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -474,187 +468,185 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>1.74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>1.84</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>1.53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>1.46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1">
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>1.53</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1">
-        <v>1.64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>1.56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>1.24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="1">
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1">
+      <c r="B17" s="4">
         <v>1.59</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2">
         <v>1.67</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="4">
         <v>1.66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2">
         <v>1.97</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="A21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="4">
         <v>1.63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>